<commit_message>
Js 8 Tugas 4 dan melengkapi semua fitur
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9AEC54-1618-4820-8CFB-B442A668919A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A458D4DA-AFB7-4FA2-AD3C-6B5B5F029388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{54818A27-3A13-4F33-B9E9-1C78F6CDF2D0}"/>
+    <workbookView xWindow="10932" yWindow="1872" windowWidth="11256" windowHeight="9420" xr2:uid="{54818A27-3A13-4F33-B9E9-1C78F6CDF2D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>